<commit_message>
image and excel update
</commit_message>
<xml_diff>
--- a/Lost_Nests_2010_2011_2012_2013_2014_2015_2016_2017_2018.xlsx
+++ b/Lost_Nests_2010_2011_2012_2013_2014_2015_2016_2017_2018.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277c80898c00dfc7/ACTIVE/UIS/Spring_2022/GEOG489/GitHub/GEOG489_Nest_Loss_Project_Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4FFAE722-8F0A-43E9-BED1-6892423D7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{4FFAE722-8F0A-43E9-BED1-6892423D7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4BE5575-2E5F-42D4-907A-D84E0EB3FAF8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lost_Nests_2010_2011_2012_2013_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -629,26 +641,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -913,10 +905,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1162,26 +1150,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1284,26 +1252,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1429,549 +1377,6 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2311,7 +1716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>